<commit_message>
:sparkles: Mochcun bot implementation
now bot example is about my business
</commit_message>
<xml_diff>
--- a/chats/clientes-saludar.xlsx
+++ b/chats/clientes-saludar.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5400" windowWidth="28800" windowHeight="12465"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet sheetId="1" name="Hoja1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -15,9 +15,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="00000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
@@ -47,9 +44,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -68,7 +64,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -84,7 +80,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -96,7 +92,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -143,6 +139,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -178,6 +191,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -332,17 +362,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>